<commit_message>
update record sampling analysis
</commit_message>
<xml_diff>
--- a/analyses/3-record-sampling/sample.xlsx
+++ b/analyses/3-record-sampling/sample.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:E201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2960,6 +2960,2506 @@
         <v>1</v>
       </c>
     </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>5094042</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>fl:be_ln:freborg-2</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Ben</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Freborg</t>
+        </is>
+      </c>
+      <c r="E102" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>7943413</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>fl:sh_ln:wakabayashi-16</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Shuichi</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Wakabayashi</t>
+        </is>
+      </c>
+      <c r="E103" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>9529934</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>fl:ka_ln:xu-94</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Kang</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Xu</t>
+        </is>
+      </c>
+      <c r="E104" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>6260281</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>fl:mi_ln:niinomi-1</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Mitsuyoshi</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Niinomi</t>
+        </is>
+      </c>
+      <c r="E105" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>7127302</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>fl:jo_ln:palm-3</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Jochen</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Palm</t>
+        </is>
+      </c>
+      <c r="E106" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>8132691</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>fl:th_ln:meinardi-1</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Thomas Roger</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Meinardi</t>
+        </is>
+      </c>
+      <c r="E107" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>4159234</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>fl:ra_ln:eifler-1</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Raymond J.</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Eifler</t>
+        </is>
+      </c>
+      <c r="E108" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>6692356</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>fl:la_ln:peterson-8</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Lance L.</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>Peterson</t>
+        </is>
+      </c>
+      <c r="E109" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>6351808</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>fl:jo_ln:chamdani-2</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Joseph I.</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Chamdani</t>
+        </is>
+      </c>
+      <c r="E110" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>10398487</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>fl:ju_ln:wang-160</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Juan</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Wang</t>
+        </is>
+      </c>
+      <c r="E111" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>6859823</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>fl:te_ln:watanabe-28</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Tetsuya</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Watanabe</t>
+        </is>
+      </c>
+      <c r="E112" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>10061147</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>fl:xi_ln:zhou-228</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Xingyao</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Zhou</t>
+        </is>
+      </c>
+      <c r="E113" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>8976983</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>fl:je_ln:seo-72</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Jeongil</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Seo</t>
+        </is>
+      </c>
+      <c r="E114" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>4873993</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>fl:th_ln:palmieri-1</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Thomas</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Palmieri</t>
+        </is>
+      </c>
+      <c r="E115" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>11172531</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>fl:ju_ln:li-150</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Junyi</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Li</t>
+        </is>
+      </c>
+      <c r="E116" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>8298552</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>fl:ma_ln:kumar-23</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Mahesh</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Kumar</t>
+        </is>
+      </c>
+      <c r="E117" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>9768696</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>fl:we_ln:zhao-226</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Wenqiang</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>Zhao</t>
+        </is>
+      </c>
+      <c r="E118" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>5120225</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>fl:no_ln:amit-3</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Amit</t>
+        </is>
+      </c>
+      <c r="E119" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>6172278</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>fl:ka_ln:georgopoulos-1</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Katia</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>Georgopoulos</t>
+        </is>
+      </c>
+      <c r="E120" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>10253479</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>fl:hi_ln:satake-4</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Hidetoshi</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>Satake</t>
+        </is>
+      </c>
+      <c r="E121" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>8597892</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>fl:ke_ln:kelnar-1</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Kevin</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Kelnar</t>
+        </is>
+      </c>
+      <c r="E122" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>7262658</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>fl:ja_ln:krishnan-10</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>Jagadeesh</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>Krishnan</t>
+        </is>
+      </c>
+      <c r="E123" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>10459662</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>fl:ma_ln:banse-2</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Mark Anthony</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>Banse</t>
+        </is>
+      </c>
+      <c r="E124" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>5792064</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>fl:do_ln:panescu-2</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Dorin</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>Panescu</t>
+        </is>
+      </c>
+      <c r="E125" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>5148159</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>fl:br_ln:martel-1</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Brian J.</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>Martel</t>
+        </is>
+      </c>
+      <c r="E126" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>4563025</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>fl:ja_ln:poe-1</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Jack L.</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>Poe</t>
+        </is>
+      </c>
+      <c r="E127" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>7209292</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>fl:al_ln:epple-1</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Alexander</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>Epple</t>
+        </is>
+      </c>
+      <c r="E128" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>8988837</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>fl:je_ln:wavering-2</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Jeffrey T.</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>Wavering</t>
+        </is>
+      </c>
+      <c r="E129" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>9054421</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>fl:ja_ln:anguerapros-3</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Jaume</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>Anguera Pros</t>
+        </is>
+      </c>
+      <c r="E130" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>11009110</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>fl:fr_ln:barillot-1</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>François</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Barillot</t>
+        </is>
+      </c>
+      <c r="E131" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>10414160</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>fl:ke_ln:hirai-17</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Keita</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>Hirai</t>
+        </is>
+      </c>
+      <c r="E132" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>9426715</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>fl:yu_ln:kim-126</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Yun Sung</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>Kim</t>
+        </is>
+      </c>
+      <c r="E133" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>9008391</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>fl:ka_ln:solanki-1</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Kaushal Mohanlal</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>Solanki</t>
+        </is>
+      </c>
+      <c r="E134" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>10835935</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>fl:ge_ln:literski-1</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Geoffrey Grant</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>Literski</t>
+        </is>
+      </c>
+      <c r="E135" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>8411651</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>fl:ca_ln:livet-1</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>Catherine M.</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>Livet</t>
+        </is>
+      </c>
+      <c r="E136" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>7155763</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>fl:to_ln:north-4</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>Toya J.</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>North</t>
+        </is>
+      </c>
+      <c r="E137" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>6147498</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>fl:os_ln:sumiya-1</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Osamu</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>Sumiya</t>
+        </is>
+      </c>
+      <c r="E138" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>9703888</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>fl:sr_ln:sistu-1</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Sreedhar</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>Sistu</t>
+        </is>
+      </c>
+      <c r="E139" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>8364647</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>fl:al_ln:lorbeer-1</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>Alex</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>Lorbeer</t>
+        </is>
+      </c>
+      <c r="E140" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>6548506</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>fl:ph_ln:girard-4</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Philippe</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>Girard</t>
+        </is>
+      </c>
+      <c r="E141" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>6390818</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>fl:ma_ln:ferranti-2</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Marann</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>Ferranti</t>
+        </is>
+      </c>
+      <c r="E142" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>10676727</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>fl:zh_ln:kang-10</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Zhengfang</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>Kang</t>
+        </is>
+      </c>
+      <c r="E143" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>7942227</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>fl:da_ln:arnold-24</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>David W.</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>Arnold</t>
+        </is>
+      </c>
+      <c r="E144" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>7417022</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>fl:sa_ln:milstein-2</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Sam J.</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Milstein</t>
+        </is>
+      </c>
+      <c r="E145" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>10101856</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>fl:yu_ln:chen-674</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Yu-Yen</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>Chen</t>
+        </is>
+      </c>
+      <c r="E146" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>5478147</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>fl:th_ln:brown-16</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Thomas R.</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="E147" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>8542034</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>fl:ki_ln:kato-36</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Kiyoshi</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>Kato</t>
+        </is>
+      </c>
+      <c r="E148" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>6953186</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>fl:ma_ln:segi-1</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Masaya</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>Segi</t>
+        </is>
+      </c>
+      <c r="E149" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>7451704</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>fl:vl_ln:gold-1</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Vladimir</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>Gold</t>
+        </is>
+      </c>
+      <c r="E150" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>6207399</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>fl:he_ln:hemker-2</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>Hendrik Coenraad</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>Hemker</t>
+        </is>
+      </c>
+      <c r="E151" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>7531011</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>fl:to_ln:yamasaki-19</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>Tomoo</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>Yamasaki</t>
+        </is>
+      </c>
+      <c r="E152" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>4783217</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>fl:ha_ln:robertson-4</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>Harry J.</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>Robertson</t>
+        </is>
+      </c>
+      <c r="E153" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>4055262</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>fl:la_ln:albright-3</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>Larry E.</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>Albright</t>
+        </is>
+      </c>
+      <c r="E154" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>7860249</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>fl:ja_ln:cuddihy-4</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>James William</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>Cuddihy</t>
+        </is>
+      </c>
+      <c r="E155" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>5904776</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>fl:ar_ln:donde-2</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>Arik</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>Donde</t>
+        </is>
+      </c>
+      <c r="E156" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>6133682</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>fl:ic_ln:saotome-1</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>Ichiro</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>Saotome</t>
+        </is>
+      </c>
+      <c r="E157" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>4701393</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>fl:te_ln:sueda-1</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>Tetsuo</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>Sueda</t>
+        </is>
+      </c>
+      <c r="E158" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>D251406</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>fl:ha_ln:takahashi-17</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>Hanji</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>Takahashi</t>
+        </is>
+      </c>
+      <c r="E159" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>10154529</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>fl:ji_ln:liu-1031</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>Jinhai</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>Liu</t>
+        </is>
+      </c>
+      <c r="E160" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>5834436</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>fl:we_ln:li-66</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>Wenhong</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>Li</t>
+        </is>
+      </c>
+      <c r="E161" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>10351682</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>fl:ma_ln:takeuchi-46</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>Masaki</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>Takeuchi</t>
+        </is>
+      </c>
+      <c r="E162" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>4065544</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>fl:be_ln:hamling-1</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>Bernard H.</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>Hamling</t>
+        </is>
+      </c>
+      <c r="E163" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>8443457</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>fl:ma_ln:stefik-1</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>Mark J.</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>Stefik</t>
+        </is>
+      </c>
+      <c r="E164" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>5669836</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>fl:ja_ln:hill-71</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>Jack O'Neil</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>Hill</t>
+        </is>
+      </c>
+      <c r="E165" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>8319354</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>fl:ch_ln:chou-440</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>Chien-Kang</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>Chou</t>
+        </is>
+      </c>
+      <c r="E166" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>9189660</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>fl:wi_ln:havens-2</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>William H.</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>Havens</t>
+        </is>
+      </c>
+      <c r="E167" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>4042952</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>fl:al_ln:kraybill-1</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>Albert Victor</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>Kraybill</t>
+        </is>
+      </c>
+      <c r="E168" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>5755308</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>fl:br_ln:bradshaw-1</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>Bradley D.</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>Bradshaw</t>
+        </is>
+      </c>
+      <c r="E169" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>5352714</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>fl:pa_ln:valint-2</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>Paul L.</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>Valint, Jr.</t>
+        </is>
+      </c>
+      <c r="E170" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>5792879</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>fl:th_ln:gessner-4</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>Thomas</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>Gessner</t>
+        </is>
+      </c>
+      <c r="E171" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>D401827</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>fl:ta_ln:lui-5</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>Tat Nin</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>Lui</t>
+        </is>
+      </c>
+      <c r="E172" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>5978038</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>fl:ku_ln:okada-12</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>Kunio</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>Okada</t>
+        </is>
+      </c>
+      <c r="E173" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>5074323</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>fl:ja_ln:seale-2</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>James B.</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>Seale</t>
+        </is>
+      </c>
+      <c r="E174" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>11196521</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>fl:ho_ln:noh-7</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>Hoondong</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>Noh</t>
+        </is>
+      </c>
+      <c r="E175" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>10474574</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>fl:se_ln:lee-1141</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>Seung-Beom</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>Lee</t>
+        </is>
+      </c>
+      <c r="E176" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>7851386</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>fl:an_ln:rao-48</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>Angelo</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>Rao</t>
+        </is>
+      </c>
+      <c r="E177" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>9979878</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>fl:sa_ln:shroff-3</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>Sapna A</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>Shroff</t>
+        </is>
+      </c>
+      <c r="E178" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>8204870</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>fl:mi_ln:ho-79</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>Michael M.</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>Ho</t>
+        </is>
+      </c>
+      <c r="E179" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>H537</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>fl:an_ln:buchanan-5</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>Antonio P.</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>Buchanan</t>
+        </is>
+      </c>
+      <c r="E180" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>8459841</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>fl:ti_ln:huang-174</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>Tien-Fu</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>Huang</t>
+        </is>
+      </c>
+      <c r="E181" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>10617440</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>fl:ph_ln:phisitkul-1</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>Phinit</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>Phisitkul</t>
+        </is>
+      </c>
+      <c r="E182" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>7258790</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>fl:a._ln:eversole-1</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>A. G.</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>Eversole</t>
+        </is>
+      </c>
+      <c r="E183" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>5550797</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>fl:ky_ln:suzuki-9</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>Kyoko</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>Suzuki</t>
+        </is>
+      </c>
+      <c r="E184" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>8252687</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>fl:pa_ln:singh-26</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>Pankaj</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>Singh</t>
+        </is>
+      </c>
+      <c r="E185" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>5470216</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>fl:ma_ln:saito-84</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>Masao</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>Saito</t>
+        </is>
+      </c>
+      <c r="E186" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>8269017</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>fl:we_ln:ying-18</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>Weiwen</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>Ying</t>
+        </is>
+      </c>
+      <c r="E187" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>10828208</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>fl:al_ln:fedotov-4</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>Alexander</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>Fedotov</t>
+        </is>
+      </c>
+      <c r="E188" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>11122412</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>fl:th_ln:tran-2</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>Thuyen C</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>Tran</t>
+        </is>
+      </c>
+      <c r="E189" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>5710492</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>fl:ma_ln:nishimura-46</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>Masashi</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>Nishimura</t>
+        </is>
+      </c>
+      <c r="E190" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>11155685</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>fl:ju_ln:nunez-2</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>Juan G.</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>Nunez</t>
+        </is>
+      </c>
+      <c r="E191" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>10333225</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>ktayab3qq2u4a6dqfsi15swpp</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>Sangeetha</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>Subbaraj</t>
+        </is>
+      </c>
+      <c r="E192" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>3950700</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>fl:em_ln:weisbart-1</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>Emanuel S.</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>Weisbart</t>
+        </is>
+      </c>
+      <c r="E193" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>7786129</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>fl:gy_ln:levay-2</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>György</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>Lévay</t>
+        </is>
+      </c>
+      <c r="E194" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>9200051</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>fl:ta_ln:asami-1</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>Taiji</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>Asami</t>
+        </is>
+      </c>
+      <c r="E195" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>5286095</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>fl:se_ln:campanini-1</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>Sergio</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>Campanini</t>
+        </is>
+      </c>
+      <c r="E196" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>10455291</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>fl:jo_ln:bernstein-1</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>Joseph Harold</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>Bernstein</t>
+        </is>
+      </c>
+      <c r="E197" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>5057055</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>fl:mi_ln:presseau-1</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>Michel</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>Presseau</t>
+        </is>
+      </c>
+      <c r="E198" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>6810399</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>fl:an_ln:osborn-5</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>Andrew</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>Osborn</t>
+        </is>
+      </c>
+      <c r="E199" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>9730177</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>fl:st_ln:toth-4</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>Stefan Karl</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>Toth</t>
+        </is>
+      </c>
+      <c r="E200" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>4614424</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>fl:sh_ln:watanabe-201</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>Shunji</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>Watanabe</t>
+        </is>
+      </c>
+      <c r="E201" t="n">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>